<commit_message>
EPBDS-11013 Add test table
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11013_ExternalConditions.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11013_ExternalConditions.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\demo\openl-demo\user-workspace\DEFAULT\SmartExternalCondition1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\demo\openl-demo\user-workspace\DEFAULT\EPBDS-11013_ExternalConditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5F09C6-911F-48DF-ACD7-B0CC46086777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F187303B-572D-40FD-9FF6-436D1C00C441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="690" windowWidth="23700" windowHeight="15060" xr2:uid="{F34CF891-5473-47EA-98FF-3F810BCD10E1}"/>
+    <workbookView xWindow="8835" yWindow="1140" windowWidth="23700" windowHeight="15060" xr2:uid="{F34CF891-5473-47EA-98FF-3F810BCD10E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
   <si>
     <t>aaa</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Datatype SomeType &lt;String&gt;</t>
   </si>
   <si>
-    <t>String param0</t>
-  </si>
-  <si>
     <t>Datatype State &lt;String&gt;</t>
   </si>
   <si>
@@ -131,69 +128,53 @@
     <t>value</t>
   </si>
   <si>
-    <t>SomeType someType, OptionCode param0, AlenaDatatype param1, AnotherCode param2, MyCode param3, State param4</t>
-  </si>
-  <si>
     <t>(value==cond3)&amp;&amp;(name==cond2)</t>
   </si>
   <si>
-    <t>SmartLookup Double mySmartLookup(SomeType someType, OptionCode param0, AlenaDatatype param1, AnotherCode param2, MyCode param3, State param4, Integer param333)</t>
-  </si>
-  <si>
     <t>Bla 3</t>
   </si>
   <si>
-    <t>SmartLookup String mySmartLookup(SomeType someType, OptionCode param0, AlenaDatatype param1, AnotherCode param2, MyCode param3, State param4, Integer param333)</t>
-  </si>
-  <si>
-    <t>true&amp;&amp;(length(param0)&gt;0)</t>
-  </si>
-  <si>
     <t>OptionCode param0</t>
   </si>
   <si>
-    <t>SmartLookup String mySmartLookup(SomeType someType,  AlenaDatatype param1, AnotherCode param2, MyCode param3, State param4, Integer param333, OptionCode param0,)</t>
-  </si>
-  <si>
-    <t>SmartLookup String mySmartLookup(SomeType someType,  AlenaDatatype param1, AnotherCode param2, MyCode param3, State param4, Integer param333, OptionCode param0)</t>
-  </si>
-  <si>
-    <t>true &amp;&amp; length(param0) &gt; 0</t>
-  </si>
-  <si>
-    <t>SmartLookup String mySmartLookup(SomeType someType,   OptionCode param0, AlenaDatatype param1, AnotherCode param2, MyCode param3, State param4, Integer param333)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true </t>
-  </si>
-  <si>
     <t>SmartLookup String mySmartLookup(SomeType someType, AlenaDatatype param1, AnotherCode param2, MyCode param3, State param4, Integer param333,  OptionCode param0)</t>
   </si>
   <si>
-    <t>(param1.value==cond3)&amp;&amp;(param1.name==cond2)</t>
-  </si>
-  <si>
-    <t>SomeType someType, OptionCode param0, AlenaDatatype param1, AnotherCode param2, MyCode param3, State param4, lenaDatatype param111</t>
-  </si>
-  <si>
-    <t>SomeType someType, OptionCode param0, AlenaDatatype param1, AnotherCode param2, MyCode param3, State param4, AlenaDatatype param111</t>
-  </si>
-  <si>
-    <t>(ad.value==cond3)&amp;&amp;(ad.name==cond2)</t>
-  </si>
-  <si>
     <t>SomeType someType, OptionCode param0, AlenaDatatype ad, AnotherCode param2, MyCode param3, State param4</t>
+  </si>
+  <si>
+    <t>Test mySmartLookup</t>
+  </si>
+  <si>
+    <t>someType</t>
+  </si>
+  <si>
+    <t>param1.name</t>
+  </si>
+  <si>
+    <t>param1.value</t>
+  </si>
+  <si>
+    <t>param2</t>
+  </si>
+  <si>
+    <t>param3</t>
+  </si>
+  <si>
+    <t>param4</t>
+  </si>
+  <si>
+    <t>_res_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -208,7 +189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -231,21 +212,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -560,338 +594,431 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D361A0-DA7C-4E63-B60C-3446DC9C1713}">
-  <dimension ref="B6:J38"/>
+  <dimension ref="B6:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
-      <c r="G9" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
+      <c r="G9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J9" t="s">
+      <c r="I9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G10">
+      <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="H10">
+      <c r="G10" s="1">
         <v>2</v>
       </c>
-      <c r="I10">
+      <c r="H10" s="1">
         <v>3</v>
       </c>
-      <c r="J10">
+      <c r="I10" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
+      <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G11">
+      <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="H11">
+      <c r="G11" s="1">
         <v>2</v>
       </c>
-      <c r="I11">
+      <c r="H11" s="1">
         <v>3</v>
       </c>
-      <c r="J11">
+      <c r="I11" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E12" t="s">
+      <c r="D12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G12">
+      <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="H12">
+      <c r="G12" s="1">
         <v>2</v>
       </c>
-      <c r="I12">
+      <c r="H12" s="1">
         <v>3</v>
       </c>
-      <c r="J12">
+      <c r="I12" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E13" t="s">
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="11"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F13" t="s">
+      <c r="D51" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
+      <c r="E51" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G51" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I13">
-        <v>3</v>
-      </c>
-      <c r="J13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" t="s">
-        <v>0</v>
-      </c>
-      <c r="I30" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+      <c r="H51" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>4</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F35" t="s">
-        <v>30</v>
-      </c>
-      <c r="G35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F36" t="s">
-        <v>30</v>
-      </c>
-      <c r="G36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D37" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="F7:F9"/>
+  <mergeCells count="12">
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B7:B9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>